<commit_message>
updated sprint burndown 4
</commit_message>
<xml_diff>
--- a/teamOverview/sprintBacklog/sprint_4/Sprint_Burndown_4.xlsx
+++ b/teamOverview/sprintBacklog/sprint_4/Sprint_Burndown_4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/392e16b045ef5b88/Documents/ComSci/Year 3 Sem 1/cscc01/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riaz\AppData\Local\Packages\CanonicalGroupLimited.UbuntuonWindows_79rhkp1fndgsc\LocalState\rootfs\root\Team10\teamOverview\sprintBacklog\sprint_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0E450E92-AAD5-4DBE-AD63-80C0DD8C93C3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F71B0DC7-92F0-4200-B758-6DC1962BEE61}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="6948" xr2:uid="{F286CB4B-5BE6-4C24-8DAB-0C2B82630A4E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
   <si>
     <t>Provisional</t>
   </si>
@@ -151,6 +151,45 @@
   </si>
   <si>
     <t>Riaz:4</t>
+  </si>
+  <si>
+    <t>10-Susan</t>
+  </si>
+  <si>
+    <t>20-David</t>
+  </si>
+  <si>
+    <t>21-Daivd</t>
+  </si>
+  <si>
+    <t>22b-Riaz</t>
+  </si>
+  <si>
+    <t>22c-Riaz</t>
+  </si>
+  <si>
+    <t>25-Dann</t>
+  </si>
+  <si>
+    <t>26-Dann</t>
+  </si>
+  <si>
+    <t>27-Dann</t>
+  </si>
+  <si>
+    <t>28-Dann</t>
+  </si>
+  <si>
+    <t>29-Dann</t>
+  </si>
+  <si>
+    <t>30-Dann</t>
+  </si>
+  <si>
+    <t>31-Dann</t>
+  </si>
+  <si>
+    <t>32-Dann</t>
   </si>
 </sst>
 </file>
@@ -1660,7 +1699,7 @@
   <dimension ref="A1:S38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G3"/>
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2261,24 +2300,24 @@
       </c>
     </row>
     <row r="25" spans="10:18" x14ac:dyDescent="0.3">
-      <c r="J25" s="1">
-        <v>10</v>
+      <c r="J25" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="O25" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="10:18" x14ac:dyDescent="0.3">
-      <c r="J26" s="1">
-        <v>20</v>
+      <c r="J26" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="M26" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="10:18" x14ac:dyDescent="0.3">
-      <c r="J27" s="1">
-        <v>21</v>
+      <c r="J27" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="M27" s="1">
         <v>1</v>
@@ -2287,7 +2326,7 @@
     </row>
     <row r="28" spans="10:18" x14ac:dyDescent="0.3">
       <c r="J28" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="M28" s="1">
         <v>3</v>
@@ -2295,71 +2334,71 @@
     </row>
     <row r="29" spans="10:18" x14ac:dyDescent="0.3">
       <c r="J29" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="O29" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="10:18" x14ac:dyDescent="0.3">
-      <c r="J30" s="1">
-        <v>25</v>
+      <c r="J30" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="K30" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="10:18" x14ac:dyDescent="0.3">
-      <c r="J31" s="1">
-        <v>26</v>
+      <c r="J31" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="K31" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="10:18" x14ac:dyDescent="0.3">
-      <c r="J32" s="1">
-        <v>27</v>
+      <c r="J32" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="M32" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="10:13" x14ac:dyDescent="0.3">
-      <c r="J33" s="1">
-        <v>28</v>
+      <c r="J33" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="M33" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="10:13" x14ac:dyDescent="0.3">
-      <c r="J34" s="1">
-        <v>29</v>
+      <c r="J34" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="M34" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="10:13" x14ac:dyDescent="0.3">
-      <c r="J35" s="1">
-        <v>30</v>
+      <c r="J35" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="M35" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="10:13" x14ac:dyDescent="0.3">
-      <c r="J36" s="1">
-        <v>31</v>
+      <c r="J36" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="M36" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="10:13" x14ac:dyDescent="0.3">
-      <c r="J37" s="1">
-        <v>32</v>
+      <c r="J37" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="M37" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Added sprint reports; for actual burndown, I edited it for actual hours for my end
</commit_message>
<xml_diff>
--- a/teamOverview/sprintBacklog/sprint_4/Sprint_Burndown_4.xlsx
+++ b/teamOverview/sprintBacklog/sprint_4/Sprint_Burndown_4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riaz\AppData\Local\Packages\CanonicalGroupLimited.UbuntuonWindows_79rhkp1fndgsc\LocalState\rootfs\root\Team10\teamOverview\sprintBacklog\sprint_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dann Justin\Desktop\new\Team10\teamOverview\sprintBacklog\sprint_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F71B0DC7-92F0-4200-B758-6DC1962BEE61}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5B566EFF-E86E-4260-AB2F-34CEEB8ED3C4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="6948" xr2:uid="{F286CB4B-5BE6-4C24-8DAB-0C2B82630A4E}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="14940" windowHeight="6948" xr2:uid="{F286CB4B-5BE6-4C24-8DAB-0C2B82630A4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -516,7 +516,7 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>14</c:v>
@@ -1698,9 +1698,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2177,11 +2175,11 @@
         <v>27</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="2"/>
-        <v>14</v>
+        <f>E15-SUM(M25:M37)</f>
+        <v>20</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="2"/>
+        <f>F15-SUM(N25:N37)</f>
         <v>14</v>
       </c>
       <c r="H15" s="1">
@@ -2360,51 +2358,51 @@
       <c r="J32" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M32" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="N32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="10:14" x14ac:dyDescent="0.3">
       <c r="J33" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="M33" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="N33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="10:14" x14ac:dyDescent="0.3">
       <c r="J34" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="M34" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="N34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="10:14" x14ac:dyDescent="0.3">
       <c r="J35" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M35" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="N35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="10:14" x14ac:dyDescent="0.3">
       <c r="J36" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M36" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="N36" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="10:14" x14ac:dyDescent="0.3">
       <c r="J37" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M37" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="10:13" x14ac:dyDescent="0.3">
+      <c r="N37" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="10:14" x14ac:dyDescent="0.3">
       <c r="J38" s="1" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
completed provisional and actual for sprint 5
</commit_message>
<xml_diff>
--- a/teamOverview/sprintBacklog/sprint_4/Sprint_Burndown_4.xlsx
+++ b/teamOverview/sprintBacklog/sprint_4/Sprint_Burndown_4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dann Justin\Desktop\new\Team10\teamOverview\sprintBacklog\sprint_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Riaz\AppData\Local\Packages\CanonicalGroupLimited.UbuntuonWindows_79rhkp1fndgsc\LocalState\rootfs\root\Team10\teamOverview\sprintBacklog\sprint_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5B566EFF-E86E-4260-AB2F-34CEEB8ED3C4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CFFF8337-DE34-4180-B776-353E2B128EBB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="14940" windowHeight="6948" xr2:uid="{F286CB4B-5BE6-4C24-8DAB-0C2B82630A4E}"/>
   </bookViews>
@@ -312,7 +312,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-CA" baseline="0"/>
-              <a:t> 3 Burdown Chart</a:t>
+              <a:t> 4 Burdown Chart</a:t>
             </a:r>
             <a:endParaRPr lang="en-CA"/>
           </a:p>
@@ -1698,7 +1698,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>